<commit_message>
All Methods added in DriverScript
</commit_message>
<xml_diff>
--- a/ERP_Hybrid/FileOutput/HybridResults.xlsx
+++ b/ERP_Hybrid/FileOutput/HybridResults.xlsx
@@ -40,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="722" uniqueCount="154">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="719" uniqueCount="153">
   <si>
     <t>TCID</t>
   </si>
@@ -499,9 +499,6 @@
   </si>
   <si>
     <t>Pass</t>
-  </si>
-  <si>
-    <t>Fail</t>
   </si>
 </sst>
 </file>
@@ -509,7 +506,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="0"/>
-  <fonts count="211" x14ac:knownFonts="1">
+  <fonts count="208" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -942,847 +939,829 @@
     <font>
       <name val="Calibri"/>
       <sz val="11.0"/>
-      <color indexed="10"/>
-      <b val="true"/>
-    </font>
-    <font>
-      <name val="Calibri"/>
-      <sz val="11.0"/>
-      <color indexed="17"/>
-      <b val="true"/>
-    </font>
-    <font>
-      <name val="Calibri"/>
-      <sz val="11.0"/>
-      <color indexed="10"/>
-      <b val="true"/>
-    </font>
-    <font>
-      <name val="Calibri"/>
-      <sz val="11.0"/>
-      <color indexed="17"/>
-      <b val="true"/>
-    </font>
-    <font>
-      <name val="Calibri"/>
-      <sz val="11.0"/>
-      <color indexed="17"/>
-      <b val="true"/>
-    </font>
-    <font>
-      <name val="Calibri"/>
-      <sz val="11.0"/>
-      <color indexed="17"/>
-      <b val="true"/>
-    </font>
-    <font>
-      <name val="Calibri"/>
-      <sz val="11.0"/>
-      <color indexed="17"/>
-      <b val="true"/>
-    </font>
-    <font>
-      <name val="Calibri"/>
-      <sz val="11.0"/>
-      <color indexed="17"/>
-      <b val="true"/>
-    </font>
-    <font>
-      <name val="Calibri"/>
-      <sz val="11.0"/>
-      <color indexed="17"/>
-      <b val="true"/>
-    </font>
-    <font>
-      <name val="Calibri"/>
-      <sz val="11.0"/>
-      <color indexed="17"/>
-      <b val="true"/>
-    </font>
-    <font>
-      <name val="Calibri"/>
-      <sz val="11.0"/>
-      <color indexed="17"/>
-      <b val="true"/>
-    </font>
-    <font>
-      <name val="Calibri"/>
-      <sz val="11.0"/>
-      <color indexed="17"/>
-      <b val="true"/>
-    </font>
-    <font>
-      <name val="Calibri"/>
-      <sz val="11.0"/>
-      <color indexed="17"/>
-      <b val="true"/>
-    </font>
-    <font>
-      <name val="Calibri"/>
-      <sz val="11.0"/>
-      <color indexed="17"/>
-      <b val="true"/>
-    </font>
-    <font>
-      <name val="Calibri"/>
-      <sz val="11.0"/>
-      <color indexed="10"/>
-      <b val="true"/>
-    </font>
-    <font>
-      <name val="Calibri"/>
-      <sz val="11.0"/>
-      <color indexed="17"/>
-      <b val="true"/>
-    </font>
-    <font>
-      <name val="Calibri"/>
-      <sz val="11.0"/>
-      <color indexed="17"/>
-      <b val="true"/>
-    </font>
-    <font>
-      <name val="Calibri"/>
-      <sz val="11.0"/>
-      <color indexed="17"/>
-      <b val="true"/>
-    </font>
-    <font>
-      <name val="Calibri"/>
-      <sz val="11.0"/>
-      <color indexed="17"/>
-      <b val="true"/>
-    </font>
-    <font>
-      <name val="Calibri"/>
-      <sz val="11.0"/>
-      <color indexed="17"/>
-      <b val="true"/>
-    </font>
-    <font>
-      <name val="Calibri"/>
-      <sz val="11.0"/>
-      <color indexed="17"/>
-      <b val="true"/>
-    </font>
-    <font>
-      <name val="Calibri"/>
-      <sz val="11.0"/>
-      <color indexed="17"/>
-      <b val="true"/>
-    </font>
-    <font>
-      <name val="Calibri"/>
-      <sz val="11.0"/>
-      <color indexed="17"/>
-      <b val="true"/>
-    </font>
-    <font>
-      <name val="Calibri"/>
-      <sz val="11.0"/>
-      <color indexed="17"/>
-      <b val="true"/>
-    </font>
-    <font>
-      <name val="Calibri"/>
-      <sz val="11.0"/>
-      <color indexed="17"/>
-      <b val="true"/>
-    </font>
-    <font>
-      <name val="Calibri"/>
-      <sz val="11.0"/>
-      <color indexed="17"/>
-      <b val="true"/>
-    </font>
-    <font>
-      <name val="Calibri"/>
-      <sz val="11.0"/>
-      <color indexed="17"/>
-      <b val="true"/>
-    </font>
-    <font>
-      <name val="Calibri"/>
-      <sz val="11.0"/>
-      <color indexed="17"/>
-      <b val="true"/>
-    </font>
-    <font>
-      <name val="Calibri"/>
-      <sz val="11.0"/>
-      <color indexed="17"/>
-      <b val="true"/>
-    </font>
-    <font>
-      <name val="Calibri"/>
-      <sz val="11.0"/>
-      <color indexed="17"/>
-      <b val="true"/>
-    </font>
-    <font>
-      <name val="Calibri"/>
-      <sz val="11.0"/>
-      <color indexed="17"/>
-      <b val="true"/>
-    </font>
-    <font>
-      <name val="Calibri"/>
-      <sz val="11.0"/>
-      <color indexed="17"/>
-      <b val="true"/>
-    </font>
-    <font>
-      <name val="Calibri"/>
-      <sz val="11.0"/>
-      <color indexed="17"/>
-      <b val="true"/>
-    </font>
-    <font>
-      <name val="Calibri"/>
-      <sz val="11.0"/>
-      <color indexed="17"/>
-      <b val="true"/>
-    </font>
-    <font>
-      <name val="Calibri"/>
-      <sz val="11.0"/>
-      <color indexed="17"/>
-      <b val="true"/>
-    </font>
-    <font>
-      <name val="Calibri"/>
-      <sz val="11.0"/>
-      <color indexed="17"/>
-      <b val="true"/>
-    </font>
-    <font>
-      <name val="Calibri"/>
-      <sz val="11.0"/>
-      <color indexed="17"/>
-      <b val="true"/>
-    </font>
-    <font>
-      <name val="Calibri"/>
-      <sz val="11.0"/>
-      <color indexed="17"/>
-      <b val="true"/>
-    </font>
-    <font>
-      <name val="Calibri"/>
-      <sz val="11.0"/>
-      <color indexed="17"/>
-      <b val="true"/>
-    </font>
-    <font>
-      <name val="Calibri"/>
-      <sz val="11.0"/>
-      <color indexed="17"/>
-      <b val="true"/>
-    </font>
-    <font>
-      <name val="Calibri"/>
-      <sz val="11.0"/>
-      <color indexed="17"/>
-      <b val="true"/>
-    </font>
-    <font>
-      <name val="Calibri"/>
-      <sz val="11.0"/>
-      <color indexed="17"/>
-      <b val="true"/>
-    </font>
-    <font>
-      <name val="Calibri"/>
-      <sz val="11.0"/>
-      <color indexed="17"/>
-      <b val="true"/>
-    </font>
-    <font>
-      <name val="Calibri"/>
-      <sz val="11.0"/>
-      <color indexed="17"/>
-      <b val="true"/>
-    </font>
-    <font>
-      <name val="Calibri"/>
-      <sz val="11.0"/>
-      <color indexed="17"/>
-      <b val="true"/>
-    </font>
-    <font>
-      <name val="Calibri"/>
-      <sz val="11.0"/>
-      <color indexed="17"/>
-      <b val="true"/>
-    </font>
-    <font>
-      <name val="Calibri"/>
-      <sz val="11.0"/>
-      <color indexed="17"/>
-      <b val="true"/>
-    </font>
-    <font>
-      <name val="Calibri"/>
-      <sz val="11.0"/>
-      <color indexed="17"/>
-      <b val="true"/>
-    </font>
-    <font>
-      <name val="Calibri"/>
-      <sz val="11.0"/>
-      <color indexed="17"/>
-      <b val="true"/>
-    </font>
-    <font>
-      <name val="Calibri"/>
-      <sz val="11.0"/>
-      <color indexed="17"/>
-      <b val="true"/>
-    </font>
-    <font>
-      <name val="Calibri"/>
-      <sz val="11.0"/>
-      <color indexed="17"/>
-      <b val="true"/>
-    </font>
-    <font>
-      <name val="Calibri"/>
-      <sz val="11.0"/>
-      <color indexed="17"/>
-      <b val="true"/>
-    </font>
-    <font>
-      <name val="Calibri"/>
-      <sz val="11.0"/>
-      <color indexed="17"/>
-      <b val="true"/>
-    </font>
-    <font>
-      <name val="Calibri"/>
-      <sz val="11.0"/>
-      <color indexed="17"/>
-      <b val="true"/>
-    </font>
-    <font>
-      <name val="Calibri"/>
-      <sz val="11.0"/>
-      <color indexed="17"/>
-      <b val="true"/>
-    </font>
-    <font>
-      <name val="Calibri"/>
-      <sz val="11.0"/>
-      <color indexed="17"/>
-      <b val="true"/>
-    </font>
-    <font>
-      <name val="Calibri"/>
-      <sz val="11.0"/>
-      <color indexed="17"/>
-      <b val="true"/>
-    </font>
-    <font>
-      <name val="Calibri"/>
-      <sz val="11.0"/>
-      <color indexed="17"/>
-      <b val="true"/>
-    </font>
-    <font>
-      <name val="Calibri"/>
-      <sz val="11.0"/>
-      <color indexed="17"/>
-      <b val="true"/>
-    </font>
-    <font>
-      <name val="Calibri"/>
-      <sz val="11.0"/>
-      <color indexed="17"/>
-      <b val="true"/>
-    </font>
-    <font>
-      <name val="Calibri"/>
-      <sz val="11.0"/>
-      <color indexed="17"/>
-      <b val="true"/>
-    </font>
-    <font>
-      <name val="Calibri"/>
-      <sz val="11.0"/>
-      <color indexed="17"/>
-      <b val="true"/>
-    </font>
-    <font>
-      <name val="Calibri"/>
-      <sz val="11.0"/>
-      <color indexed="17"/>
-      <b val="true"/>
-    </font>
-    <font>
-      <name val="Calibri"/>
-      <sz val="11.0"/>
-      <color indexed="17"/>
-      <b val="true"/>
-    </font>
-    <font>
-      <name val="Calibri"/>
-      <sz val="11.0"/>
-      <color indexed="17"/>
-      <b val="true"/>
-    </font>
-    <font>
-      <name val="Calibri"/>
-      <sz val="11.0"/>
-      <color indexed="17"/>
-      <b val="true"/>
-    </font>
-    <font>
-      <name val="Calibri"/>
-      <sz val="11.0"/>
-      <color indexed="17"/>
-      <b val="true"/>
-    </font>
-    <font>
-      <name val="Calibri"/>
-      <sz val="11.0"/>
-      <color indexed="17"/>
-      <b val="true"/>
-    </font>
-    <font>
-      <name val="Calibri"/>
-      <sz val="11.0"/>
-      <color indexed="17"/>
-      <b val="true"/>
-    </font>
-    <font>
-      <name val="Calibri"/>
-      <sz val="11.0"/>
-      <color indexed="17"/>
-      <b val="true"/>
-    </font>
-    <font>
-      <name val="Calibri"/>
-      <sz val="11.0"/>
-      <color indexed="17"/>
-      <b val="true"/>
-    </font>
-    <font>
-      <name val="Calibri"/>
-      <sz val="11.0"/>
-      <color indexed="17"/>
-      <b val="true"/>
-    </font>
-    <font>
-      <name val="Calibri"/>
-      <sz val="11.0"/>
-      <color indexed="17"/>
-      <b val="true"/>
-    </font>
-    <font>
-      <name val="Calibri"/>
-      <sz val="11.0"/>
-      <color indexed="17"/>
-      <b val="true"/>
-    </font>
-    <font>
-      <name val="Calibri"/>
-      <sz val="11.0"/>
-      <color indexed="17"/>
-      <b val="true"/>
-    </font>
-    <font>
-      <name val="Calibri"/>
-      <sz val="11.0"/>
-      <color indexed="17"/>
-      <b val="true"/>
-    </font>
-    <font>
-      <name val="Calibri"/>
-      <sz val="11.0"/>
-      <color indexed="17"/>
-      <b val="true"/>
-    </font>
-    <font>
-      <name val="Calibri"/>
-      <sz val="11.0"/>
-      <color indexed="10"/>
-      <b val="true"/>
-    </font>
-    <font>
-      <name val="Calibri"/>
-      <sz val="11.0"/>
-      <color indexed="17"/>
-      <b val="true"/>
-    </font>
-    <font>
-      <name val="Calibri"/>
-      <sz val="11.0"/>
-      <color indexed="17"/>
-      <b val="true"/>
-    </font>
-    <font>
-      <name val="Calibri"/>
-      <sz val="11.0"/>
-      <color indexed="17"/>
-      <b val="true"/>
-    </font>
-    <font>
-      <name val="Calibri"/>
-      <sz val="11.0"/>
-      <color indexed="17"/>
-      <b val="true"/>
-    </font>
-    <font>
-      <name val="Calibri"/>
-      <sz val="11.0"/>
-      <color indexed="17"/>
-      <b val="true"/>
-    </font>
-    <font>
-      <name val="Calibri"/>
-      <sz val="11.0"/>
-      <color indexed="17"/>
-      <b val="true"/>
-    </font>
-    <font>
-      <name val="Calibri"/>
-      <sz val="11.0"/>
-      <color indexed="17"/>
-      <b val="true"/>
-    </font>
-    <font>
-      <name val="Calibri"/>
-      <sz val="11.0"/>
-      <color indexed="17"/>
-      <b val="true"/>
-    </font>
-    <font>
-      <name val="Calibri"/>
-      <sz val="11.0"/>
-      <color indexed="17"/>
-      <b val="true"/>
-    </font>
-    <font>
-      <name val="Calibri"/>
-      <sz val="11.0"/>
-      <color indexed="17"/>
-      <b val="true"/>
-    </font>
-    <font>
-      <name val="Calibri"/>
-      <sz val="11.0"/>
-      <color indexed="17"/>
-      <b val="true"/>
-    </font>
-    <font>
-      <name val="Calibri"/>
-      <sz val="11.0"/>
-      <color indexed="17"/>
-      <b val="true"/>
-    </font>
-    <font>
-      <name val="Calibri"/>
-      <sz val="11.0"/>
-      <color indexed="17"/>
-      <b val="true"/>
-    </font>
-    <font>
-      <name val="Calibri"/>
-      <sz val="11.0"/>
-      <color indexed="17"/>
-      <b val="true"/>
-    </font>
-    <font>
-      <name val="Calibri"/>
-      <sz val="11.0"/>
-      <color indexed="17"/>
-      <b val="true"/>
-    </font>
-    <font>
-      <name val="Calibri"/>
-      <sz val="11.0"/>
-      <color indexed="17"/>
-      <b val="true"/>
-    </font>
-    <font>
-      <name val="Calibri"/>
-      <sz val="11.0"/>
-      <color indexed="17"/>
-      <b val="true"/>
-    </font>
-    <font>
-      <name val="Calibri"/>
-      <sz val="11.0"/>
-      <color indexed="17"/>
-      <b val="true"/>
-    </font>
-    <font>
-      <name val="Calibri"/>
-      <sz val="11.0"/>
-      <color indexed="17"/>
-      <b val="true"/>
-    </font>
-    <font>
-      <name val="Calibri"/>
-      <sz val="11.0"/>
-      <color indexed="17"/>
-      <b val="true"/>
-    </font>
-    <font>
-      <name val="Calibri"/>
-      <sz val="11.0"/>
-      <color indexed="17"/>
-      <b val="true"/>
-    </font>
-    <font>
-      <name val="Calibri"/>
-      <sz val="11.0"/>
-      <color indexed="17"/>
-      <b val="true"/>
-    </font>
-    <font>
-      <name val="Calibri"/>
-      <sz val="11.0"/>
-      <color indexed="17"/>
-      <b val="true"/>
-    </font>
-    <font>
-      <name val="Calibri"/>
-      <sz val="11.0"/>
-      <color indexed="17"/>
-      <b val="true"/>
-    </font>
-    <font>
-      <name val="Calibri"/>
-      <sz val="11.0"/>
-      <color indexed="17"/>
-      <b val="true"/>
-    </font>
-    <font>
-      <name val="Calibri"/>
-      <sz val="11.0"/>
-      <color indexed="17"/>
-      <b val="true"/>
-    </font>
-    <font>
-      <name val="Calibri"/>
-      <sz val="11.0"/>
-      <color indexed="17"/>
-      <b val="true"/>
-    </font>
-    <font>
-      <name val="Calibri"/>
-      <sz val="11.0"/>
-      <color indexed="17"/>
-      <b val="true"/>
-    </font>
-    <font>
-      <name val="Calibri"/>
-      <sz val="11.0"/>
-      <color indexed="17"/>
-      <b val="true"/>
-    </font>
-    <font>
-      <name val="Calibri"/>
-      <sz val="11.0"/>
-      <color indexed="17"/>
-      <b val="true"/>
-    </font>
-    <font>
-      <name val="Calibri"/>
-      <sz val="11.0"/>
-      <color indexed="17"/>
-      <b val="true"/>
-    </font>
-    <font>
-      <name val="Calibri"/>
-      <sz val="11.0"/>
-      <color indexed="17"/>
-      <b val="true"/>
-    </font>
-    <font>
-      <name val="Calibri"/>
-      <sz val="11.0"/>
-      <color indexed="17"/>
-      <b val="true"/>
-    </font>
-    <font>
-      <name val="Calibri"/>
-      <sz val="11.0"/>
-      <color indexed="17"/>
-      <b val="true"/>
-    </font>
-    <font>
-      <name val="Calibri"/>
-      <sz val="11.0"/>
-      <color indexed="17"/>
-      <b val="true"/>
-    </font>
-    <font>
-      <name val="Calibri"/>
-      <sz val="11.0"/>
-      <color indexed="17"/>
-      <b val="true"/>
-    </font>
-    <font>
-      <name val="Calibri"/>
-      <sz val="11.0"/>
-      <color indexed="17"/>
-      <b val="true"/>
-    </font>
-    <font>
-      <name val="Calibri"/>
-      <sz val="11.0"/>
-      <color indexed="17"/>
-      <b val="true"/>
-    </font>
-    <font>
-      <name val="Calibri"/>
-      <sz val="11.0"/>
-      <color indexed="17"/>
-      <b val="true"/>
-    </font>
-    <font>
-      <name val="Calibri"/>
-      <sz val="11.0"/>
-      <color indexed="17"/>
-      <b val="true"/>
-    </font>
-    <font>
-      <name val="Calibri"/>
-      <sz val="11.0"/>
-      <color indexed="17"/>
-      <b val="true"/>
-    </font>
-    <font>
-      <name val="Calibri"/>
-      <sz val="11.0"/>
-      <color indexed="17"/>
-      <b val="true"/>
-    </font>
-    <font>
-      <name val="Calibri"/>
-      <sz val="11.0"/>
-      <color indexed="17"/>
-      <b val="true"/>
-    </font>
-    <font>
-      <name val="Calibri"/>
-      <sz val="11.0"/>
-      <color indexed="17"/>
-      <b val="true"/>
-    </font>
-    <font>
-      <name val="Calibri"/>
-      <sz val="11.0"/>
-      <color indexed="17"/>
-      <b val="true"/>
-    </font>
-    <font>
-      <name val="Calibri"/>
-      <sz val="11.0"/>
-      <color indexed="17"/>
-      <b val="true"/>
-    </font>
-    <font>
-      <name val="Calibri"/>
-      <sz val="11.0"/>
-      <color indexed="17"/>
-      <b val="true"/>
-    </font>
-    <font>
-      <name val="Calibri"/>
-      <sz val="11.0"/>
-      <color indexed="17"/>
-      <b val="true"/>
-    </font>
-    <font>
-      <name val="Calibri"/>
-      <sz val="11.0"/>
-      <color indexed="17"/>
-      <b val="true"/>
-    </font>
-    <font>
-      <name val="Calibri"/>
-      <sz val="11.0"/>
-      <color indexed="17"/>
-      <b val="true"/>
-    </font>
-    <font>
-      <name val="Calibri"/>
-      <sz val="11.0"/>
-      <color indexed="17"/>
-      <b val="true"/>
-    </font>
-    <font>
-      <name val="Calibri"/>
-      <sz val="11.0"/>
-      <color indexed="17"/>
-      <b val="true"/>
-    </font>
-    <font>
-      <name val="Calibri"/>
-      <sz val="11.0"/>
-      <color indexed="17"/>
-      <b val="true"/>
-    </font>
-    <font>
-      <name val="Calibri"/>
-      <sz val="11.0"/>
-      <color indexed="17"/>
-      <b val="true"/>
-    </font>
-    <font>
-      <name val="Calibri"/>
-      <sz val="11.0"/>
-      <color indexed="17"/>
-      <b val="true"/>
-    </font>
-    <font>
-      <name val="Calibri"/>
-      <sz val="11.0"/>
-      <color indexed="17"/>
-      <b val="true"/>
-    </font>
-    <font>
-      <name val="Calibri"/>
-      <sz val="11.0"/>
-      <color indexed="17"/>
-      <b val="true"/>
-    </font>
-    <font>
-      <name val="Calibri"/>
-      <sz val="11.0"/>
-      <color indexed="17"/>
-      <b val="true"/>
-    </font>
-    <font>
-      <name val="Calibri"/>
-      <sz val="11.0"/>
-      <color indexed="17"/>
-      <b val="true"/>
-    </font>
-    <font>
-      <name val="Calibri"/>
-      <sz val="11.0"/>
-      <color indexed="17"/>
-      <b val="true"/>
-    </font>
-    <font>
-      <name val="Calibri"/>
-      <sz val="11.0"/>
-      <color indexed="17"/>
-      <b val="true"/>
-    </font>
-    <font>
-      <name val="Calibri"/>
-      <sz val="11.0"/>
-      <color indexed="17"/>
-      <b val="true"/>
-    </font>
-    <font>
-      <name val="Calibri"/>
-      <sz val="11.0"/>
-      <color indexed="10"/>
+      <color indexed="17"/>
+      <b val="true"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+      <color indexed="17"/>
+      <b val="true"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+      <color indexed="17"/>
+      <b val="true"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+      <color indexed="17"/>
+      <b val="true"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+      <color indexed="17"/>
+      <b val="true"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+      <color indexed="17"/>
+      <b val="true"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+      <color indexed="17"/>
+      <b val="true"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+      <color indexed="17"/>
+      <b val="true"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+      <color indexed="17"/>
+      <b val="true"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+      <color indexed="17"/>
+      <b val="true"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+      <color indexed="17"/>
+      <b val="true"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+      <color indexed="17"/>
+      <b val="true"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+      <color indexed="17"/>
+      <b val="true"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+      <color indexed="17"/>
+      <b val="true"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+      <color indexed="17"/>
+      <b val="true"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+      <color indexed="17"/>
+      <b val="true"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+      <color indexed="17"/>
+      <b val="true"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+      <color indexed="17"/>
+      <b val="true"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+      <color indexed="17"/>
+      <b val="true"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+      <color indexed="17"/>
+      <b val="true"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+      <color indexed="17"/>
+      <b val="true"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+      <color indexed="17"/>
+      <b val="true"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+      <color indexed="17"/>
+      <b val="true"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+      <color indexed="17"/>
+      <b val="true"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+      <color indexed="17"/>
+      <b val="true"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+      <color indexed="17"/>
+      <b val="true"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+      <color indexed="17"/>
+      <b val="true"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+      <color indexed="17"/>
+      <b val="true"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+      <color indexed="17"/>
+      <b val="true"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+      <color indexed="17"/>
+      <b val="true"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+      <color indexed="17"/>
+      <b val="true"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+      <color indexed="17"/>
+      <b val="true"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+      <color indexed="17"/>
+      <b val="true"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+      <color indexed="17"/>
+      <b val="true"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+      <color indexed="17"/>
+      <b val="true"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+      <color indexed="17"/>
+      <b val="true"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+      <color indexed="17"/>
+      <b val="true"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+      <color indexed="17"/>
+      <b val="true"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+      <color indexed="17"/>
+      <b val="true"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+      <color indexed="17"/>
+      <b val="true"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+      <color indexed="17"/>
+      <b val="true"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+      <color indexed="17"/>
+      <b val="true"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+      <color indexed="17"/>
+      <b val="true"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+      <color indexed="17"/>
+      <b val="true"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+      <color indexed="17"/>
+      <b val="true"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+      <color indexed="17"/>
+      <b val="true"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+      <color indexed="17"/>
+      <b val="true"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+      <color indexed="17"/>
+      <b val="true"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+      <color indexed="17"/>
+      <b val="true"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+      <color indexed="17"/>
+      <b val="true"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+      <color indexed="17"/>
+      <b val="true"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+      <color indexed="17"/>
+      <b val="true"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+      <color indexed="17"/>
+      <b val="true"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+      <color indexed="17"/>
+      <b val="true"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+      <color indexed="17"/>
+      <b val="true"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+      <color indexed="17"/>
+      <b val="true"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+      <color indexed="17"/>
+      <b val="true"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+      <color indexed="17"/>
+      <b val="true"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+      <color indexed="17"/>
+      <b val="true"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+      <color indexed="17"/>
+      <b val="true"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+      <color indexed="17"/>
+      <b val="true"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+      <color indexed="17"/>
+      <b val="true"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+      <color indexed="17"/>
+      <b val="true"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+      <color indexed="17"/>
+      <b val="true"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+      <color indexed="17"/>
+      <b val="true"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+      <color indexed="17"/>
+      <b val="true"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+      <color indexed="17"/>
+      <b val="true"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+      <color indexed="17"/>
+      <b val="true"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+      <color indexed="17"/>
+      <b val="true"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+      <color indexed="17"/>
+      <b val="true"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+      <color indexed="17"/>
+      <b val="true"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+      <color indexed="17"/>
+      <b val="true"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+      <color indexed="17"/>
+      <b val="true"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+      <color indexed="17"/>
+      <b val="true"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+      <color indexed="17"/>
+      <b val="true"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+      <color indexed="17"/>
+      <b val="true"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+      <color indexed="17"/>
+      <b val="true"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+      <color indexed="17"/>
+      <b val="true"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+      <color indexed="17"/>
+      <b val="true"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+      <color indexed="17"/>
+      <b val="true"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+      <color indexed="17"/>
+      <b val="true"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+      <color indexed="17"/>
+      <b val="true"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+      <color indexed="17"/>
+      <b val="true"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+      <color indexed="17"/>
+      <b val="true"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+      <color indexed="17"/>
+      <b val="true"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+      <color indexed="17"/>
+      <b val="true"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+      <color indexed="17"/>
+      <b val="true"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+      <color indexed="17"/>
+      <b val="true"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+      <color indexed="17"/>
+      <b val="true"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+      <color indexed="17"/>
+      <b val="true"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+      <color indexed="17"/>
+      <b val="true"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+      <color indexed="17"/>
+      <b val="true"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+      <color indexed="17"/>
+      <b val="true"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+      <color indexed="17"/>
+      <b val="true"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+      <color indexed="17"/>
+      <b val="true"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+      <color indexed="17"/>
+      <b val="true"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+      <color indexed="17"/>
+      <b val="true"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+      <color indexed="17"/>
+      <b val="true"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+      <color indexed="17"/>
+      <b val="true"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+      <color indexed="17"/>
+      <b val="true"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+      <color indexed="17"/>
+      <b val="true"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+      <color indexed="17"/>
+      <b val="true"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+      <color indexed="17"/>
+      <b val="true"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+      <color indexed="17"/>
+      <b val="true"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+      <color indexed="17"/>
+      <b val="true"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+      <color indexed="17"/>
+      <b val="true"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+      <color indexed="17"/>
+      <b val="true"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+      <color indexed="17"/>
+      <b val="true"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+      <color indexed="17"/>
+      <b val="true"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+      <color indexed="17"/>
+      <b val="true"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+      <color indexed="17"/>
+      <b val="true"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+      <color indexed="17"/>
+      <b val="true"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+      <color indexed="17"/>
+      <b val="true"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+      <color indexed="17"/>
+      <b val="true"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+      <color indexed="17"/>
+      <b val="true"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+      <color indexed="17"/>
+      <b val="true"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+      <color indexed="17"/>
+      <b val="true"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+      <color indexed="17"/>
+      <b val="true"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+      <color indexed="17"/>
+      <b val="true"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+      <color indexed="17"/>
+      <b val="true"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+      <color indexed="17"/>
+      <b val="true"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+      <color indexed="17"/>
+      <b val="true"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+      <color indexed="17"/>
+      <b val="true"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+      <color indexed="17"/>
+      <b val="true"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+      <color indexed="17"/>
+      <b val="true"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+      <color indexed="17"/>
+      <b val="true"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+      <color indexed="17"/>
+      <b val="true"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+      <color indexed="17"/>
+      <b val="true"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+      <color indexed="17"/>
+      <b val="true"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+      <color indexed="17"/>
+      <b val="true"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+      <color indexed="17"/>
+      <b val="true"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+      <color indexed="17"/>
+      <b val="true"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+      <color indexed="17"/>
+      <b val="true"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+      <color indexed="17"/>
+      <b val="true"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+      <color indexed="17"/>
+      <b val="true"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+      <color indexed="17"/>
+      <b val="true"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+      <color indexed="17"/>
+      <b val="true"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+      <color indexed="17"/>
       <b val="true"/>
     </font>
   </fonts>
@@ -1828,7 +1807,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="214">
+  <cellXfs count="211">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
@@ -2042,9 +2021,6 @@
     <xf numFmtId="0" fontId="205" fillId="0" borderId="0" xfId="0" applyFont="true"/>
     <xf numFmtId="0" fontId="206" fillId="0" borderId="0" xfId="0" applyFont="true"/>
     <xf numFmtId="0" fontId="207" fillId="0" borderId="0" xfId="0" applyFont="true"/>
-    <xf numFmtId="0" fontId="208" fillId="0" borderId="0" xfId="0" applyFont="true"/>
-    <xf numFmtId="0" fontId="209" fillId="0" borderId="0" xfId="0" applyFont="true"/>
-    <xf numFmtId="0" fontId="210" fillId="0" borderId="0" xfId="0" applyFont="true"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -2430,8 +2406,8 @@
       <c r="C3" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="D3" t="s" s="87">
-        <v>153</v>
+      <c r="D3" t="s" s="86">
+        <v>152</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.3">
@@ -2444,8 +2420,8 @@
       <c r="C4" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="D4" t="s" s="150">
-        <v>153</v>
+      <c r="D4" t="s" s="148">
+        <v>152</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.3">
@@ -2458,8 +2434,8 @@
       <c r="C5" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="D5" t="s" s="213">
-        <v>153</v>
+      <c r="D5" t="s" s="210">
+        <v>152</v>
       </c>
     </row>
   </sheetData>
@@ -3205,7 +3181,7 @@
         <v>10</v>
       </c>
       <c r="F24" t="s" s="73">
-        <v>153</v>
+        <v>152</v>
       </c>
     </row>
     <row r="25" spans="1:6" ht="15.6" x14ac:dyDescent="0.3">
@@ -3225,7 +3201,7 @@
         <v>20</v>
       </c>
       <c r="F25" t="s" s="75">
-        <v>153</v>
+        <v>152</v>
       </c>
     </row>
     <row r="26" spans="1:6" ht="15.6" x14ac:dyDescent="0.3">
@@ -3387,7 +3363,7 @@
       <c r="E2" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="F2" t="s" s="88">
+      <c r="F2" t="s" s="87">
         <v>152</v>
       </c>
     </row>
@@ -3407,7 +3383,7 @@
       <c r="E3" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="F3" t="s" s="90">
+      <c r="F3" t="s" s="89">
         <v>152</v>
       </c>
     </row>
@@ -3427,7 +3403,7 @@
       <c r="E4" s="4">
         <v>10</v>
       </c>
-      <c r="F4" t="s" s="92">
+      <c r="F4" t="s" s="91">
         <v>152</v>
       </c>
     </row>
@@ -3447,7 +3423,7 @@
       <c r="E5" s="4" t="s">
         <v>30</v>
       </c>
-      <c r="F5" t="s" s="94">
+      <c r="F5" t="s" s="93">
         <v>152</v>
       </c>
     </row>
@@ -3467,7 +3443,7 @@
       <c r="E6" s="4" t="s">
         <v>33</v>
       </c>
-      <c r="F6" t="s" s="96">
+      <c r="F6" t="s" s="95">
         <v>152</v>
       </c>
     </row>
@@ -3487,7 +3463,7 @@
       <c r="E7" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="F7" t="s" s="98">
+      <c r="F7" t="s" s="97">
         <v>152</v>
       </c>
     </row>
@@ -3507,7 +3483,7 @@
       <c r="E8" s="4">
         <v>10</v>
       </c>
-      <c r="F8" t="s" s="100">
+      <c r="F8" t="s" s="99">
         <v>152</v>
       </c>
     </row>
@@ -3527,7 +3503,7 @@
       <c r="E9" s="4" t="s">
         <v>41</v>
       </c>
-      <c r="F9" t="s" s="102">
+      <c r="F9" t="s" s="101">
         <v>152</v>
       </c>
     </row>
@@ -3547,7 +3523,7 @@
       <c r="E10" s="6">
         <v>10</v>
       </c>
-      <c r="F10" t="s" s="104">
+      <c r="F10" t="s" s="103">
         <v>152</v>
       </c>
     </row>
@@ -3567,7 +3543,7 @@
       <c r="E11" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="F11" t="s" s="106">
+      <c r="F11" t="s" s="105">
         <v>152</v>
       </c>
     </row>
@@ -3587,7 +3563,7 @@
       <c r="E12" s="6">
         <v>10</v>
       </c>
-      <c r="F12" t="s" s="108">
+      <c r="F12" t="s" s="107">
         <v>152</v>
       </c>
     </row>
@@ -3607,7 +3583,7 @@
       <c r="E13" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="F13" t="s" s="110">
+      <c r="F13" t="s" s="109">
         <v>152</v>
       </c>
     </row>
@@ -3627,7 +3603,7 @@
       <c r="E14" s="6">
         <v>10</v>
       </c>
-      <c r="F14" t="s" s="112">
+      <c r="F14" t="s" s="111">
         <v>152</v>
       </c>
     </row>
@@ -3647,7 +3623,7 @@
       <c r="E15" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="F15" t="s" s="114">
+      <c r="F15" t="s" s="113">
         <v>152</v>
       </c>
     </row>
@@ -3667,7 +3643,7 @@
       <c r="E16" s="4" t="s">
         <v>97</v>
       </c>
-      <c r="F16" t="s" s="116">
+      <c r="F16" t="s" s="115">
         <v>152</v>
       </c>
     </row>
@@ -3687,7 +3663,7 @@
       <c r="E17" s="4" t="s">
         <v>100</v>
       </c>
-      <c r="F17" t="s" s="118">
+      <c r="F17" t="s" s="117">
         <v>152</v>
       </c>
     </row>
@@ -3707,7 +3683,7 @@
       <c r="E18" s="4" t="s">
         <v>103</v>
       </c>
-      <c r="F18" t="s" s="120">
+      <c r="F18" t="s" s="119">
         <v>152</v>
       </c>
     </row>
@@ -3727,7 +3703,7 @@
       <c r="E19" s="4" t="s">
         <v>106</v>
       </c>
-      <c r="F19" t="s" s="122">
+      <c r="F19" t="s" s="121">
         <v>152</v>
       </c>
     </row>
@@ -3747,7 +3723,7 @@
       <c r="E20" s="4" t="s">
         <v>109</v>
       </c>
-      <c r="F20" t="s" s="124">
+      <c r="F20" t="s" s="123">
         <v>152</v>
       </c>
     </row>
@@ -3767,7 +3743,7 @@
       <c r="E21" s="7" t="s">
         <v>112</v>
       </c>
-      <c r="F21" t="s" s="126">
+      <c r="F21" t="s" s="125">
         <v>152</v>
       </c>
     </row>
@@ -3787,7 +3763,7 @@
       <c r="E22" s="8" t="s">
         <v>115</v>
       </c>
-      <c r="F22" t="s" s="128">
+      <c r="F22" t="s" s="127">
         <v>152</v>
       </c>
     </row>
@@ -3807,7 +3783,7 @@
       <c r="E23" s="7" t="s">
         <v>118</v>
       </c>
-      <c r="F23" t="s" s="130">
+      <c r="F23" t="s" s="129">
         <v>152</v>
       </c>
     </row>
@@ -3827,7 +3803,7 @@
       <c r="E24" s="4" t="s">
         <v>121</v>
       </c>
-      <c r="F24" t="s" s="132">
+      <c r="F24" t="s" s="131">
         <v>152</v>
       </c>
     </row>
@@ -3847,7 +3823,7 @@
       <c r="E25" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="F25" t="s" s="134">
+      <c r="F25" t="s" s="133">
         <v>152</v>
       </c>
     </row>
@@ -3867,7 +3843,7 @@
       <c r="E26" s="4">
         <v>10</v>
       </c>
-      <c r="F26" t="s" s="136">
+      <c r="F26" t="s" s="135">
         <v>152</v>
       </c>
     </row>
@@ -3887,7 +3863,7 @@
       <c r="E27" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="F27" t="s" s="138">
+      <c r="F27" t="s" s="137">
         <v>152</v>
       </c>
     </row>
@@ -3907,7 +3883,7 @@
       <c r="E28" s="4">
         <v>10</v>
       </c>
-      <c r="F28" t="s" s="140">
+      <c r="F28" t="s" s="139">
         <v>152</v>
       </c>
     </row>
@@ -3927,7 +3903,7 @@
       <c r="E29" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="F29" t="s" s="142">
+      <c r="F29" t="s" s="141">
         <v>152</v>
       </c>
     </row>
@@ -3947,7 +3923,7 @@
       <c r="E30" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="F30" t="s" s="144">
+      <c r="F30" t="s" s="143">
         <v>152</v>
       </c>
     </row>
@@ -3967,7 +3943,7 @@
       <c r="E31" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="F31" t="s" s="146">
+      <c r="F31" t="s" s="145">
         <v>152</v>
       </c>
     </row>
@@ -3987,7 +3963,7 @@
       <c r="E32" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="F32" t="s" s="148">
+      <c r="F32" t="s" s="147">
         <v>152</v>
       </c>
     </row>
@@ -4053,7 +4029,7 @@
       <c r="E2" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="F2" t="s" s="151">
+      <c r="F2" t="s" s="149">
         <v>152</v>
       </c>
     </row>
@@ -4073,7 +4049,7 @@
       <c r="E3" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="F3" t="s" s="153">
+      <c r="F3" t="s" s="151">
         <v>152</v>
       </c>
     </row>
@@ -4093,7 +4069,7 @@
       <c r="E4" s="4">
         <v>10</v>
       </c>
-      <c r="F4" t="s" s="155">
+      <c r="F4" t="s" s="153">
         <v>152</v>
       </c>
     </row>
@@ -4113,7 +4089,7 @@
       <c r="E5" s="4" t="s">
         <v>30</v>
       </c>
-      <c r="F5" t="s" s="157">
+      <c r="F5" t="s" s="155">
         <v>152</v>
       </c>
     </row>
@@ -4133,7 +4109,7 @@
       <c r="E6" s="4" t="s">
         <v>33</v>
       </c>
-      <c r="F6" t="s" s="159">
+      <c r="F6" t="s" s="157">
         <v>152</v>
       </c>
     </row>
@@ -4153,7 +4129,7 @@
       <c r="E7" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="F7" t="s" s="161">
+      <c r="F7" t="s" s="159">
         <v>152</v>
       </c>
     </row>
@@ -4173,7 +4149,7 @@
       <c r="E8" s="4">
         <v>10</v>
       </c>
-      <c r="F8" t="s" s="163">
+      <c r="F8" t="s" s="161">
         <v>152</v>
       </c>
     </row>
@@ -4193,7 +4169,7 @@
       <c r="E9" s="4" t="s">
         <v>41</v>
       </c>
-      <c r="F9" t="s" s="165">
+      <c r="F9" t="s" s="163">
         <v>152</v>
       </c>
     </row>
@@ -4213,7 +4189,7 @@
       <c r="E10" s="6">
         <v>10</v>
       </c>
-      <c r="F10" t="s" s="167">
+      <c r="F10" t="s" s="165">
         <v>152</v>
       </c>
     </row>
@@ -4233,7 +4209,7 @@
       <c r="E11" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="F11" t="s" s="169">
+      <c r="F11" t="s" s="167">
         <v>152</v>
       </c>
     </row>
@@ -4253,7 +4229,7 @@
       <c r="E12" s="6">
         <v>10</v>
       </c>
-      <c r="F12" t="s" s="171">
+      <c r="F12" t="s" s="169">
         <v>152</v>
       </c>
     </row>
@@ -4273,7 +4249,7 @@
       <c r="E13" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="F13" t="s" s="173">
+      <c r="F13" t="s" s="171">
         <v>152</v>
       </c>
     </row>
@@ -4293,7 +4269,7 @@
       <c r="E14" s="6">
         <v>10</v>
       </c>
-      <c r="F14" t="s" s="175">
+      <c r="F14" t="s" s="173">
         <v>152</v>
       </c>
     </row>
@@ -4313,7 +4289,7 @@
       <c r="E15" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="F15" t="s" s="177">
+      <c r="F15" t="s" s="175">
         <v>152</v>
       </c>
     </row>
@@ -4333,7 +4309,7 @@
       <c r="E16" s="4" t="s">
         <v>142</v>
       </c>
-      <c r="F16" t="s" s="179">
+      <c r="F16" t="s" s="177">
         <v>152</v>
       </c>
     </row>
@@ -4353,7 +4329,7 @@
       <c r="E17" s="4" t="s">
         <v>136</v>
       </c>
-      <c r="F17" t="s" s="181">
+      <c r="F17" t="s" s="179">
         <v>152</v>
       </c>
     </row>
@@ -4373,7 +4349,7 @@
       <c r="E18" s="4" t="s">
         <v>103</v>
       </c>
-      <c r="F18" t="s" s="183">
+      <c r="F18" t="s" s="181">
         <v>152</v>
       </c>
     </row>
@@ -4393,7 +4369,7 @@
       <c r="E19" s="4" t="s">
         <v>106</v>
       </c>
-      <c r="F19" t="s" s="185">
+      <c r="F19" t="s" s="183">
         <v>152</v>
       </c>
     </row>
@@ -4413,7 +4389,7 @@
       <c r="E20" s="4" t="s">
         <v>109</v>
       </c>
-      <c r="F20" t="s" s="187">
+      <c r="F20" t="s" s="185">
         <v>152</v>
       </c>
     </row>
@@ -4433,7 +4409,7 @@
       <c r="E21" s="7" t="s">
         <v>112</v>
       </c>
-      <c r="F21" t="s" s="189">
+      <c r="F21" t="s" s="187">
         <v>152</v>
       </c>
     </row>
@@ -4453,7 +4429,7 @@
       <c r="E22" s="8" t="s">
         <v>137</v>
       </c>
-      <c r="F22" t="s" s="191">
+      <c r="F22" t="s" s="189">
         <v>152</v>
       </c>
     </row>
@@ -4473,7 +4449,7 @@
       <c r="E23" s="7" t="s">
         <v>118</v>
       </c>
-      <c r="F23" t="s" s="193">
+      <c r="F23" t="s" s="191">
         <v>152</v>
       </c>
     </row>
@@ -4493,7 +4469,7 @@
       <c r="E24" s="4" t="s">
         <v>138</v>
       </c>
-      <c r="F24" t="s" s="195">
+      <c r="F24" t="s" s="193">
         <v>152</v>
       </c>
     </row>
@@ -4513,7 +4489,7 @@
       <c r="E25" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="F25" t="s" s="197">
+      <c r="F25" t="s" s="195">
         <v>152</v>
       </c>
     </row>
@@ -4533,7 +4509,7 @@
       <c r="E26" s="4">
         <v>10</v>
       </c>
-      <c r="F26" t="s" s="199">
+      <c r="F26" t="s" s="197">
         <v>152</v>
       </c>
     </row>
@@ -4553,7 +4529,7 @@
       <c r="E27" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="F27" t="s" s="201">
+      <c r="F27" t="s" s="199">
         <v>152</v>
       </c>
     </row>
@@ -4573,7 +4549,7 @@
       <c r="E28" s="4">
         <v>10</v>
       </c>
-      <c r="F28" t="s" s="203">
+      <c r="F28" t="s" s="201">
         <v>152</v>
       </c>
     </row>
@@ -4593,7 +4569,7 @@
       <c r="E29" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="F29" t="s" s="205">
+      <c r="F29" t="s" s="203">
         <v>152</v>
       </c>
     </row>
@@ -4613,7 +4589,7 @@
       <c r="E30" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="F30" t="s" s="207">
+      <c r="F30" t="s" s="205">
         <v>152</v>
       </c>
     </row>
@@ -4633,7 +4609,7 @@
       <c r="E31" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="F31" t="s" s="209">
+      <c r="F31" t="s" s="207">
         <v>152</v>
       </c>
     </row>
@@ -4653,7 +4629,7 @@
       <c r="E32" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="F32" t="s" s="211">
+      <c r="F32" t="s" s="209">
         <v>152</v>
       </c>
     </row>

</xml_diff>